<commit_message>
add TUM SMT and BIO_ECONOMICS
</commit_message>
<xml_diff>
--- a/api/python/TaiGerTranscriptAnalyzerJS/database/Management/MGM_Course_database.xlsx
+++ b/api/python/TaiGerTranscriptAnalyzerJS/database/Management/MGM_Course_database.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>所有科目</t>
   </si>
@@ -233,6 +233,18 @@
   <si>
     <t>Microeconomics</t>
   </si>
+  <si>
+    <t>循環經濟</t>
+  </si>
+  <si>
+    <t>Circular Economy</t>
+  </si>
+  <si>
+    <t>永續發展</t>
+  </si>
+  <si>
+    <t>Sustainable Development</t>
+  </si>
 </sst>
 </file>
 
@@ -298,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -321,6 +333,18 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1669,10 +1693,10 @@
       <c r="Z35" s="2"/>
     </row>
     <row r="36">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="8" t="s">
         <v>71</v>
       </c>
       <c r="C36" s="2"/>
@@ -1701,8 +1725,12 @@
       <c r="Z36" s="2"/>
     </row>
     <row r="37">
-      <c r="A37" s="4"/>
-      <c r="B37" s="6"/>
+      <c r="A37" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>73</v>
+      </c>
       <c r="C37" s="2"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -1729,8 +1757,12 @@
       <c r="Z37" s="2"/>
     </row>
     <row r="38">
-      <c r="A38" s="4"/>
-      <c r="B38" s="6"/>
+      <c r="A38" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>75</v>
+      </c>
       <c r="C38" s="2"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
@@ -1758,7 +1790,7 @@
     </row>
     <row r="39">
       <c r="A39" s="4"/>
-      <c r="B39" s="6"/>
+      <c r="B39" s="11"/>
       <c r="C39" s="2"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -1786,7 +1818,7 @@
     </row>
     <row r="40">
       <c r="A40" s="4"/>
-      <c r="B40" s="6"/>
+      <c r="B40" s="11"/>
       <c r="C40" s="2"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -1814,7 +1846,7 @@
     </row>
     <row r="41">
       <c r="A41" s="4"/>
-      <c r="B41" s="6"/>
+      <c r="B41" s="11"/>
       <c r="C41" s="2"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
@@ -1842,7 +1874,7 @@
     </row>
     <row r="42">
       <c r="A42" s="4"/>
-      <c r="B42" s="6"/>
+      <c r="B42" s="11"/>
       <c r="C42" s="2"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
@@ -1870,7 +1902,7 @@
     </row>
     <row r="43">
       <c r="A43" s="4"/>
-      <c r="B43" s="6"/>
+      <c r="B43" s="11"/>
       <c r="C43" s="2"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
@@ -1898,7 +1930,7 @@
     </row>
     <row r="44">
       <c r="A44" s="4"/>
-      <c r="B44" s="6"/>
+      <c r="B44" s="11"/>
       <c r="C44" s="2"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
@@ -1926,7 +1958,7 @@
     </row>
     <row r="45">
       <c r="A45" s="4"/>
-      <c r="B45" s="6"/>
+      <c r="B45" s="11"/>
       <c r="C45" s="2"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
@@ -1954,7 +1986,7 @@
     </row>
     <row r="46">
       <c r="A46" s="4"/>
-      <c r="B46" s="6"/>
+      <c r="B46" s="11"/>
       <c r="C46" s="2"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
@@ -1982,7 +2014,7 @@
     </row>
     <row r="47">
       <c r="A47" s="4"/>
-      <c r="B47" s="6"/>
+      <c r="B47" s="11"/>
       <c r="C47" s="2"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
@@ -2010,7 +2042,7 @@
     </row>
     <row r="48">
       <c r="A48" s="4"/>
-      <c r="B48" s="6"/>
+      <c r="B48" s="11"/>
       <c r="C48" s="2"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
@@ -6657,7 +6689,7 @@
       <c r="Z213" s="2"/>
     </row>
     <row r="214">
-      <c r="A214" s="8"/>
+      <c r="A214" s="12"/>
       <c r="B214" s="6"/>
       <c r="C214" s="6"/>
       <c r="D214" s="6"/>

</xml_diff>

<commit_message>
fix manager course analysis button, modifying application overview page (not finished yet
</commit_message>
<xml_diff>
--- a/api/python/TaiGerTranscriptAnalyzerJS/database/Management/MGM_Course_database.xlsx
+++ b/api/python/TaiGerTranscriptAnalyzerJS/database/Management/MGM_Course_database.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>所有科目</t>
   </si>
@@ -245,6 +245,12 @@
   <si>
     <t>Sustainable Development</t>
   </si>
+  <si>
+    <t>綠色經濟</t>
+  </si>
+  <si>
+    <t>Green Economy</t>
+  </si>
 </sst>
 </file>
 
@@ -310,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -343,6 +349,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1789,8 +1798,12 @@
       <c r="Z38" s="2"/>
     </row>
     <row r="39">
-      <c r="A39" s="4"/>
-      <c r="B39" s="11"/>
+      <c r="A39" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>77</v>
+      </c>
       <c r="C39" s="2"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -1818,7 +1831,7 @@
     </row>
     <row r="40">
       <c r="A40" s="4"/>
-      <c r="B40" s="11"/>
+      <c r="B40" s="12"/>
       <c r="C40" s="2"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -1846,7 +1859,7 @@
     </row>
     <row r="41">
       <c r="A41" s="4"/>
-      <c r="B41" s="11"/>
+      <c r="B41" s="12"/>
       <c r="C41" s="2"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
@@ -1874,7 +1887,7 @@
     </row>
     <row r="42">
       <c r="A42" s="4"/>
-      <c r="B42" s="11"/>
+      <c r="B42" s="12"/>
       <c r="C42" s="2"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
@@ -1902,7 +1915,7 @@
     </row>
     <row r="43">
       <c r="A43" s="4"/>
-      <c r="B43" s="11"/>
+      <c r="B43" s="12"/>
       <c r="C43" s="2"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
@@ -1930,7 +1943,7 @@
     </row>
     <row r="44">
       <c r="A44" s="4"/>
-      <c r="B44" s="11"/>
+      <c r="B44" s="12"/>
       <c r="C44" s="2"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
@@ -1958,7 +1971,7 @@
     </row>
     <row r="45">
       <c r="A45" s="4"/>
-      <c r="B45" s="11"/>
+      <c r="B45" s="12"/>
       <c r="C45" s="2"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
@@ -1986,7 +1999,7 @@
     </row>
     <row r="46">
       <c r="A46" s="4"/>
-      <c r="B46" s="11"/>
+      <c r="B46" s="12"/>
       <c r="C46" s="2"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
@@ -2014,7 +2027,7 @@
     </row>
     <row r="47">
       <c r="A47" s="4"/>
-      <c r="B47" s="11"/>
+      <c r="B47" s="12"/>
       <c r="C47" s="2"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
@@ -2042,7 +2055,7 @@
     </row>
     <row r="48">
       <c r="A48" s="4"/>
-      <c r="B48" s="11"/>
+      <c r="B48" s="12"/>
       <c r="C48" s="2"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
@@ -6689,7 +6702,7 @@
       <c r="Z213" s="2"/>
     </row>
     <row r="214">
-      <c r="A214" s="12"/>
+      <c r="A214" s="13"/>
       <c r="B214" s="6"/>
       <c r="C214" s="6"/>
       <c r="D214" s="6"/>

</xml_diff>

<commit_message>
improve mgm course analysis, add ireland etc new countries, add chinese text email weekly reminder
</commit_message>
<xml_diff>
--- a/api/python/TaiGerTranscriptAnalyzerJS/database/Management/MGM_Course_database.xlsx
+++ b/api/python/TaiGerTranscriptAnalyzerJS/database/Management/MGM_Course_database.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="IBrcZ9oCBUk2FJEXEquNDlrPaJYWN4f+rAxn55kEXcU="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="aJPw6Uds2Pkf9vlh6YGWIb6R4DB4Sh6f7xFkCMg4IVU="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>所有科目</t>
   </si>
@@ -234,6 +234,30 @@
     <t>Microeconomics</t>
   </si>
   <si>
+    <t>財政學</t>
+  </si>
+  <si>
+    <t>Public Finance</t>
+  </si>
+  <si>
+    <t>政治經濟學</t>
+  </si>
+  <si>
+    <t>Political Economy</t>
+  </si>
+  <si>
+    <t>金融經濟學</t>
+  </si>
+  <si>
+    <t>Finance Economics</t>
+  </si>
+  <si>
+    <t>經濟政策與應用</t>
+  </si>
+  <si>
+    <t>Economic Policy Application</t>
+  </si>
+  <si>
     <t>循環經濟</t>
   </si>
   <si>
@@ -316,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -345,13 +369,16 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+      <alignment horizontal="left" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
@@ -1545,7 +1572,7 @@
       <c r="A31" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="8" t="s">
         <v>61</v>
       </c>
       <c r="C31" s="2"/>
@@ -1577,7 +1604,7 @@
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="8" t="s">
         <v>63</v>
       </c>
       <c r="C32" s="2"/>
@@ -1609,7 +1636,7 @@
       <c r="A33" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="8" t="s">
         <v>65</v>
       </c>
       <c r="C33" s="2"/>
@@ -1641,7 +1668,7 @@
       <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="8" t="s">
         <v>67</v>
       </c>
       <c r="C34" s="2"/>
@@ -1673,7 +1700,7 @@
       <c r="A35" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="8" t="s">
         <v>69</v>
       </c>
       <c r="C35" s="2"/>
@@ -1737,7 +1764,7 @@
       <c r="A37" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="9" t="s">
         <v>73</v>
       </c>
       <c r="C37" s="2"/>
@@ -1766,10 +1793,10 @@
       <c r="Z37" s="2"/>
     </row>
     <row r="38">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="11" t="s">
         <v>75</v>
       </c>
       <c r="C38" s="2"/>
@@ -1798,10 +1825,10 @@
       <c r="Z38" s="2"/>
     </row>
     <row r="39">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="9" t="s">
         <v>77</v>
       </c>
       <c r="C39" s="2"/>
@@ -1830,8 +1857,12 @@
       <c r="Z39" s="2"/>
     </row>
     <row r="40">
-      <c r="A40" s="4"/>
-      <c r="B40" s="12"/>
+      <c r="A40" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>79</v>
+      </c>
       <c r="C40" s="2"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -1851,15 +1882,19 @@
       <c r="S40" s="6"/>
       <c r="T40" s="6"/>
       <c r="U40" s="6"/>
-      <c r="V40" s="6"/>
+      <c r="V40" s="3"/>
       <c r="W40" s="2"/>
       <c r="X40" s="2"/>
       <c r="Y40" s="2"/>
       <c r="Z40" s="2"/>
     </row>
     <row r="41">
-      <c r="A41" s="4"/>
-      <c r="B41" s="12"/>
+      <c r="A41" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>81</v>
+      </c>
       <c r="C41" s="2"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
@@ -1879,15 +1914,19 @@
       <c r="S41" s="6"/>
       <c r="T41" s="6"/>
       <c r="U41" s="6"/>
-      <c r="V41" s="3"/>
+      <c r="V41" s="6"/>
       <c r="W41" s="2"/>
       <c r="X41" s="2"/>
       <c r="Y41" s="2"/>
       <c r="Z41" s="2"/>
     </row>
     <row r="42">
-      <c r="A42" s="4"/>
-      <c r="B42" s="12"/>
+      <c r="A42" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>83</v>
+      </c>
       <c r="C42" s="2"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
@@ -1907,15 +1946,19 @@
       <c r="S42" s="6"/>
       <c r="T42" s="6"/>
       <c r="U42" s="6"/>
-      <c r="V42" s="3"/>
+      <c r="V42" s="6"/>
       <c r="W42" s="2"/>
       <c r="X42" s="2"/>
       <c r="Y42" s="2"/>
       <c r="Z42" s="2"/>
     </row>
     <row r="43">
-      <c r="A43" s="4"/>
-      <c r="B43" s="12"/>
+      <c r="A43" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>85</v>
+      </c>
       <c r="C43" s="2"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
@@ -1935,7 +1978,7 @@
       <c r="S43" s="6"/>
       <c r="T43" s="6"/>
       <c r="U43" s="6"/>
-      <c r="V43" s="3"/>
+      <c r="V43" s="6"/>
       <c r="W43" s="2"/>
       <c r="X43" s="2"/>
       <c r="Y43" s="2"/>
@@ -1943,7 +1986,7 @@
     </row>
     <row r="44">
       <c r="A44" s="4"/>
-      <c r="B44" s="12"/>
+      <c r="B44" s="13"/>
       <c r="C44" s="2"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
@@ -1971,7 +2014,7 @@
     </row>
     <row r="45">
       <c r="A45" s="4"/>
-      <c r="B45" s="12"/>
+      <c r="B45" s="13"/>
       <c r="C45" s="2"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
@@ -1999,7 +2042,7 @@
     </row>
     <row r="46">
       <c r="A46" s="4"/>
-      <c r="B46" s="12"/>
+      <c r="B46" s="13"/>
       <c r="C46" s="2"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
@@ -2027,7 +2070,7 @@
     </row>
     <row r="47">
       <c r="A47" s="4"/>
-      <c r="B47" s="12"/>
+      <c r="B47" s="13"/>
       <c r="C47" s="2"/>
       <c r="D47" s="6"/>
       <c r="E47" s="6"/>
@@ -2055,7 +2098,7 @@
     </row>
     <row r="48">
       <c r="A48" s="4"/>
-      <c r="B48" s="12"/>
+      <c r="B48" s="13"/>
       <c r="C48" s="2"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
@@ -2083,7 +2126,7 @@
     </row>
     <row r="49">
       <c r="A49" s="4"/>
-      <c r="B49" s="6"/>
+      <c r="B49" s="13"/>
       <c r="C49" s="2"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
@@ -2111,7 +2154,7 @@
     </row>
     <row r="50">
       <c r="A50" s="4"/>
-      <c r="B50" s="6"/>
+      <c r="B50" s="13"/>
       <c r="C50" s="2"/>
       <c r="D50" s="6"/>
       <c r="E50" s="6"/>
@@ -2215,7 +2258,7 @@
       <c r="S53" s="6"/>
       <c r="T53" s="6"/>
       <c r="U53" s="6"/>
-      <c r="V53" s="6"/>
+      <c r="V53" s="3"/>
       <c r="W53" s="2"/>
       <c r="X53" s="2"/>
       <c r="Y53" s="2"/>
@@ -2243,7 +2286,7 @@
       <c r="S54" s="6"/>
       <c r="T54" s="6"/>
       <c r="U54" s="6"/>
-      <c r="V54" s="6"/>
+      <c r="V54" s="3"/>
       <c r="W54" s="2"/>
       <c r="X54" s="2"/>
       <c r="Y54" s="2"/>
@@ -2782,7 +2825,7 @@
       <c r="Z73" s="2"/>
     </row>
     <row r="74">
-      <c r="A74" s="2"/>
+      <c r="A74" s="4"/>
       <c r="B74" s="6"/>
       <c r="C74" s="2"/>
       <c r="D74" s="6"/>
@@ -2810,7 +2853,7 @@
       <c r="Z74" s="2"/>
     </row>
     <row r="75">
-      <c r="A75" s="2"/>
+      <c r="A75" s="4"/>
       <c r="B75" s="6"/>
       <c r="C75" s="2"/>
       <c r="D75" s="6"/>
@@ -2831,7 +2874,7 @@
       <c r="S75" s="6"/>
       <c r="T75" s="6"/>
       <c r="U75" s="6"/>
-      <c r="V75" s="3"/>
+      <c r="V75" s="6"/>
       <c r="W75" s="2"/>
       <c r="X75" s="2"/>
       <c r="Y75" s="2"/>
@@ -2859,7 +2902,7 @@
       <c r="S76" s="6"/>
       <c r="T76" s="6"/>
       <c r="U76" s="6"/>
-      <c r="V76" s="3"/>
+      <c r="V76" s="6"/>
       <c r="W76" s="2"/>
       <c r="X76" s="2"/>
       <c r="Y76" s="2"/>
@@ -2943,7 +2986,7 @@
       <c r="S79" s="6"/>
       <c r="T79" s="6"/>
       <c r="U79" s="6"/>
-      <c r="V79" s="6"/>
+      <c r="V79" s="3"/>
       <c r="W79" s="2"/>
       <c r="X79" s="2"/>
       <c r="Y79" s="2"/>
@@ -2971,7 +3014,7 @@
       <c r="S80" s="6"/>
       <c r="T80" s="6"/>
       <c r="U80" s="6"/>
-      <c r="V80" s="6"/>
+      <c r="V80" s="3"/>
       <c r="W80" s="2"/>
       <c r="X80" s="2"/>
       <c r="Y80" s="2"/>
@@ -2999,7 +3042,7 @@
       <c r="S81" s="6"/>
       <c r="T81" s="6"/>
       <c r="U81" s="6"/>
-      <c r="V81" s="3"/>
+      <c r="V81" s="6"/>
       <c r="W81" s="2"/>
       <c r="X81" s="2"/>
       <c r="Y81" s="2"/>
@@ -3027,7 +3070,7 @@
       <c r="S82" s="6"/>
       <c r="T82" s="6"/>
       <c r="U82" s="6"/>
-      <c r="V82" s="3"/>
+      <c r="V82" s="6"/>
       <c r="W82" s="2"/>
       <c r="X82" s="2"/>
       <c r="Y82" s="2"/>
@@ -3139,7 +3182,7 @@
       <c r="S86" s="6"/>
       <c r="T86" s="6"/>
       <c r="U86" s="6"/>
-      <c r="V86" s="6"/>
+      <c r="V86" s="3"/>
       <c r="W86" s="2"/>
       <c r="X86" s="2"/>
       <c r="Y86" s="2"/>
@@ -3167,7 +3210,7 @@
       <c r="S87" s="6"/>
       <c r="T87" s="6"/>
       <c r="U87" s="6"/>
-      <c r="V87" s="6"/>
+      <c r="V87" s="3"/>
       <c r="W87" s="2"/>
       <c r="X87" s="2"/>
       <c r="Y87" s="2"/>
@@ -3428,7 +3471,7 @@
     <row r="97">
       <c r="A97" s="2"/>
       <c r="B97" s="6"/>
-      <c r="C97" s="6"/>
+      <c r="C97" s="2"/>
       <c r="D97" s="6"/>
       <c r="E97" s="6"/>
       <c r="F97" s="2"/>
@@ -3456,7 +3499,7 @@
     <row r="98">
       <c r="A98" s="2"/>
       <c r="B98" s="6"/>
-      <c r="C98" s="6"/>
+      <c r="C98" s="2"/>
       <c r="D98" s="6"/>
       <c r="E98" s="6"/>
       <c r="F98" s="2"/>
@@ -3587,7 +3630,7 @@
       <c r="S102" s="6"/>
       <c r="T102" s="6"/>
       <c r="U102" s="6"/>
-      <c r="V102" s="3"/>
+      <c r="V102" s="6"/>
       <c r="W102" s="2"/>
       <c r="X102" s="2"/>
       <c r="Y102" s="2"/>
@@ -3615,7 +3658,7 @@
       <c r="S103" s="6"/>
       <c r="T103" s="6"/>
       <c r="U103" s="6"/>
-      <c r="V103" s="3"/>
+      <c r="V103" s="6"/>
       <c r="W103" s="2"/>
       <c r="X103" s="2"/>
       <c r="Y103" s="2"/>
@@ -3643,7 +3686,7 @@
       <c r="S104" s="6"/>
       <c r="T104" s="6"/>
       <c r="U104" s="6"/>
-      <c r="V104" s="6"/>
+      <c r="V104" s="3"/>
       <c r="W104" s="2"/>
       <c r="X104" s="2"/>
       <c r="Y104" s="2"/>
@@ -3671,7 +3714,7 @@
       <c r="S105" s="6"/>
       <c r="T105" s="6"/>
       <c r="U105" s="6"/>
-      <c r="V105" s="6"/>
+      <c r="V105" s="3"/>
       <c r="W105" s="2"/>
       <c r="X105" s="2"/>
       <c r="Y105" s="2"/>
@@ -3811,7 +3854,7 @@
       <c r="S110" s="6"/>
       <c r="T110" s="6"/>
       <c r="U110" s="6"/>
-      <c r="V110" s="3"/>
+      <c r="V110" s="6"/>
       <c r="W110" s="2"/>
       <c r="X110" s="2"/>
       <c r="Y110" s="2"/>
@@ -3839,7 +3882,7 @@
       <c r="S111" s="6"/>
       <c r="T111" s="6"/>
       <c r="U111" s="6"/>
-      <c r="V111" s="3"/>
+      <c r="V111" s="6"/>
       <c r="W111" s="2"/>
       <c r="X111" s="2"/>
       <c r="Y111" s="2"/>
@@ -3867,7 +3910,7 @@
       <c r="S112" s="6"/>
       <c r="T112" s="6"/>
       <c r="U112" s="6"/>
-      <c r="V112" s="6"/>
+      <c r="V112" s="3"/>
       <c r="W112" s="2"/>
       <c r="X112" s="2"/>
       <c r="Y112" s="2"/>
@@ -3895,7 +3938,7 @@
       <c r="S113" s="6"/>
       <c r="T113" s="6"/>
       <c r="U113" s="6"/>
-      <c r="V113" s="6"/>
+      <c r="V113" s="3"/>
       <c r="W113" s="2"/>
       <c r="X113" s="2"/>
       <c r="Y113" s="2"/>
@@ -4091,7 +4134,7 @@
       <c r="S120" s="6"/>
       <c r="T120" s="6"/>
       <c r="U120" s="6"/>
-      <c r="V120" s="3"/>
+      <c r="V120" s="6"/>
       <c r="W120" s="2"/>
       <c r="X120" s="2"/>
       <c r="Y120" s="2"/>
@@ -4119,7 +4162,7 @@
       <c r="S121" s="6"/>
       <c r="T121" s="6"/>
       <c r="U121" s="6"/>
-      <c r="V121" s="3"/>
+      <c r="V121" s="6"/>
       <c r="W121" s="2"/>
       <c r="X121" s="2"/>
       <c r="Y121" s="2"/>
@@ -4371,7 +4414,7 @@
       <c r="S130" s="6"/>
       <c r="T130" s="6"/>
       <c r="U130" s="6"/>
-      <c r="V130" s="6"/>
+      <c r="V130" s="3"/>
       <c r="W130" s="2"/>
       <c r="X130" s="2"/>
       <c r="Y130" s="2"/>
@@ -4399,7 +4442,7 @@
       <c r="S131" s="6"/>
       <c r="T131" s="6"/>
       <c r="U131" s="6"/>
-      <c r="V131" s="6"/>
+      <c r="V131" s="3"/>
       <c r="W131" s="2"/>
       <c r="X131" s="2"/>
       <c r="Y131" s="2"/>
@@ -4427,7 +4470,7 @@
       <c r="S132" s="6"/>
       <c r="T132" s="6"/>
       <c r="U132" s="6"/>
-      <c r="V132" s="3"/>
+      <c r="V132" s="6"/>
       <c r="W132" s="2"/>
       <c r="X132" s="2"/>
       <c r="Y132" s="2"/>
@@ -4483,7 +4526,7 @@
       <c r="S134" s="6"/>
       <c r="T134" s="6"/>
       <c r="U134" s="6"/>
-      <c r="V134" s="6"/>
+      <c r="V134" s="3"/>
       <c r="W134" s="2"/>
       <c r="X134" s="2"/>
       <c r="Y134" s="2"/>
@@ -4511,7 +4554,7 @@
       <c r="S135" s="6"/>
       <c r="T135" s="6"/>
       <c r="U135" s="6"/>
-      <c r="V135" s="3"/>
+      <c r="V135" s="6"/>
       <c r="W135" s="2"/>
       <c r="X135" s="2"/>
       <c r="Y135" s="2"/>
@@ -4539,7 +4582,7 @@
       <c r="S136" s="6"/>
       <c r="T136" s="6"/>
       <c r="U136" s="6"/>
-      <c r="V136" s="3"/>
+      <c r="V136" s="6"/>
       <c r="W136" s="2"/>
       <c r="X136" s="2"/>
       <c r="Y136" s="2"/>
@@ -4763,7 +4806,7 @@
       <c r="S144" s="6"/>
       <c r="T144" s="6"/>
       <c r="U144" s="6"/>
-      <c r="V144" s="6"/>
+      <c r="V144" s="3"/>
       <c r="W144" s="2"/>
       <c r="X144" s="2"/>
       <c r="Y144" s="2"/>
@@ -4791,7 +4834,7 @@
       <c r="S145" s="6"/>
       <c r="T145" s="6"/>
       <c r="U145" s="6"/>
-      <c r="V145" s="6"/>
+      <c r="V145" s="3"/>
       <c r="W145" s="2"/>
       <c r="X145" s="2"/>
       <c r="Y145" s="2"/>
@@ -4819,7 +4862,7 @@
       <c r="S146" s="6"/>
       <c r="T146" s="6"/>
       <c r="U146" s="6"/>
-      <c r="V146" s="3"/>
+      <c r="V146" s="6"/>
       <c r="W146" s="2"/>
       <c r="X146" s="2"/>
       <c r="Y146" s="2"/>
@@ -4875,7 +4918,7 @@
       <c r="S148" s="6"/>
       <c r="T148" s="6"/>
       <c r="U148" s="6"/>
-      <c r="V148" s="6"/>
+      <c r="V148" s="3"/>
       <c r="W148" s="2"/>
       <c r="X148" s="2"/>
       <c r="Y148" s="2"/>
@@ -4931,7 +4974,7 @@
       <c r="S150" s="6"/>
       <c r="T150" s="6"/>
       <c r="U150" s="6"/>
-      <c r="V150" s="3"/>
+      <c r="V150" s="6"/>
       <c r="W150" s="2"/>
       <c r="X150" s="2"/>
       <c r="Y150" s="2"/>
@@ -4959,7 +5002,7 @@
       <c r="S151" s="6"/>
       <c r="T151" s="6"/>
       <c r="U151" s="6"/>
-      <c r="V151" s="3"/>
+      <c r="V151" s="6"/>
       <c r="W151" s="2"/>
       <c r="X151" s="2"/>
       <c r="Y151" s="2"/>
@@ -4987,7 +5030,7 @@
       <c r="S152" s="6"/>
       <c r="T152" s="6"/>
       <c r="U152" s="6"/>
-      <c r="V152" s="6"/>
+      <c r="V152" s="3"/>
       <c r="W152" s="2"/>
       <c r="X152" s="2"/>
       <c r="Y152" s="2"/>
@@ -5015,7 +5058,7 @@
       <c r="S153" s="6"/>
       <c r="T153" s="6"/>
       <c r="U153" s="6"/>
-      <c r="V153" s="6"/>
+      <c r="V153" s="3"/>
       <c r="W153" s="2"/>
       <c r="X153" s="2"/>
       <c r="Y153" s="2"/>
@@ -5435,7 +5478,7 @@
       <c r="S168" s="6"/>
       <c r="T168" s="6"/>
       <c r="U168" s="6"/>
-      <c r="V168" s="3"/>
+      <c r="V168" s="6"/>
       <c r="W168" s="2"/>
       <c r="X168" s="2"/>
       <c r="Y168" s="2"/>
@@ -5463,7 +5506,7 @@
       <c r="S169" s="6"/>
       <c r="T169" s="6"/>
       <c r="U169" s="6"/>
-      <c r="V169" s="3"/>
+      <c r="V169" s="6"/>
       <c r="W169" s="2"/>
       <c r="X169" s="2"/>
       <c r="Y169" s="2"/>
@@ -5491,7 +5534,7 @@
       <c r="S170" s="6"/>
       <c r="T170" s="6"/>
       <c r="U170" s="6"/>
-      <c r="V170" s="6"/>
+      <c r="V170" s="3"/>
       <c r="W170" s="2"/>
       <c r="X170" s="2"/>
       <c r="Y170" s="2"/>
@@ -5519,7 +5562,7 @@
       <c r="S171" s="6"/>
       <c r="T171" s="6"/>
       <c r="U171" s="6"/>
-      <c r="V171" s="6"/>
+      <c r="V171" s="3"/>
       <c r="W171" s="2"/>
       <c r="X171" s="2"/>
       <c r="Y171" s="2"/>
@@ -5547,7 +5590,7 @@
       <c r="S172" s="6"/>
       <c r="T172" s="6"/>
       <c r="U172" s="6"/>
-      <c r="V172" s="3"/>
+      <c r="V172" s="6"/>
       <c r="W172" s="2"/>
       <c r="X172" s="2"/>
       <c r="Y172" s="2"/>
@@ -5575,7 +5618,7 @@
       <c r="S173" s="6"/>
       <c r="T173" s="6"/>
       <c r="U173" s="6"/>
-      <c r="V173" s="3"/>
+      <c r="V173" s="6"/>
       <c r="W173" s="2"/>
       <c r="X173" s="2"/>
       <c r="Y173" s="2"/>
@@ -5603,7 +5646,7 @@
       <c r="S174" s="6"/>
       <c r="T174" s="6"/>
       <c r="U174" s="6"/>
-      <c r="V174" s="6"/>
+      <c r="V174" s="3"/>
       <c r="W174" s="2"/>
       <c r="X174" s="2"/>
       <c r="Y174" s="2"/>
@@ -5631,7 +5674,7 @@
       <c r="S175" s="6"/>
       <c r="T175" s="6"/>
       <c r="U175" s="6"/>
-      <c r="V175" s="6"/>
+      <c r="V175" s="3"/>
       <c r="W175" s="2"/>
       <c r="X175" s="2"/>
       <c r="Y175" s="2"/>
@@ -6051,7 +6094,7 @@
       <c r="S190" s="6"/>
       <c r="T190" s="6"/>
       <c r="U190" s="6"/>
-      <c r="V190" s="3"/>
+      <c r="V190" s="6"/>
       <c r="W190" s="2"/>
       <c r="X190" s="2"/>
       <c r="Y190" s="2"/>
@@ -6079,7 +6122,7 @@
       <c r="S191" s="6"/>
       <c r="T191" s="6"/>
       <c r="U191" s="6"/>
-      <c r="V191" s="3"/>
+      <c r="V191" s="6"/>
       <c r="W191" s="2"/>
       <c r="X191" s="2"/>
       <c r="Y191" s="2"/>
@@ -6163,7 +6206,7 @@
       <c r="S194" s="6"/>
       <c r="T194" s="6"/>
       <c r="U194" s="6"/>
-      <c r="V194" s="6"/>
+      <c r="V194" s="3"/>
       <c r="W194" s="2"/>
       <c r="X194" s="2"/>
       <c r="Y194" s="2"/>
@@ -6191,7 +6234,7 @@
       <c r="S195" s="6"/>
       <c r="T195" s="6"/>
       <c r="U195" s="6"/>
-      <c r="V195" s="6"/>
+      <c r="V195" s="3"/>
       <c r="W195" s="2"/>
       <c r="X195" s="2"/>
       <c r="Y195" s="2"/>
@@ -6275,7 +6318,7 @@
       <c r="S198" s="6"/>
       <c r="T198" s="6"/>
       <c r="U198" s="6"/>
-      <c r="V198" s="3"/>
+      <c r="V198" s="6"/>
       <c r="W198" s="2"/>
       <c r="X198" s="2"/>
       <c r="Y198" s="2"/>
@@ -6303,7 +6346,7 @@
       <c r="S199" s="6"/>
       <c r="T199" s="6"/>
       <c r="U199" s="6"/>
-      <c r="V199" s="3"/>
+      <c r="V199" s="6"/>
       <c r="W199" s="2"/>
       <c r="X199" s="2"/>
       <c r="Y199" s="2"/>
@@ -6331,7 +6374,7 @@
       <c r="S200" s="6"/>
       <c r="T200" s="6"/>
       <c r="U200" s="6"/>
-      <c r="V200" s="6"/>
+      <c r="V200" s="3"/>
       <c r="W200" s="2"/>
       <c r="X200" s="2"/>
       <c r="Y200" s="2"/>
@@ -6359,7 +6402,7 @@
       <c r="S201" s="6"/>
       <c r="T201" s="6"/>
       <c r="U201" s="6"/>
-      <c r="V201" s="6"/>
+      <c r="V201" s="3"/>
       <c r="W201" s="2"/>
       <c r="X201" s="2"/>
       <c r="Y201" s="2"/>
@@ -6611,7 +6654,7 @@
       <c r="S210" s="6"/>
       <c r="T210" s="6"/>
       <c r="U210" s="6"/>
-      <c r="V210" s="3"/>
+      <c r="V210" s="6"/>
       <c r="W210" s="2"/>
       <c r="X210" s="2"/>
       <c r="Y210" s="2"/>
@@ -6639,7 +6682,7 @@
       <c r="S211" s="6"/>
       <c r="T211" s="6"/>
       <c r="U211" s="6"/>
-      <c r="V211" s="3"/>
+      <c r="V211" s="6"/>
       <c r="W211" s="2"/>
       <c r="X211" s="2"/>
       <c r="Y211" s="2"/>
@@ -6667,7 +6710,7 @@
       <c r="S212" s="6"/>
       <c r="T212" s="6"/>
       <c r="U212" s="6"/>
-      <c r="V212" s="6"/>
+      <c r="V212" s="3"/>
       <c r="W212" s="2"/>
       <c r="X212" s="2"/>
       <c r="Y212" s="2"/>
@@ -6695,14 +6738,14 @@
       <c r="S213" s="6"/>
       <c r="T213" s="6"/>
       <c r="U213" s="6"/>
-      <c r="V213" s="6"/>
+      <c r="V213" s="3"/>
       <c r="W213" s="2"/>
       <c r="X213" s="2"/>
       <c r="Y213" s="2"/>
       <c r="Z213" s="2"/>
     </row>
     <row r="214">
-      <c r="A214" s="13"/>
+      <c r="A214" s="2"/>
       <c r="B214" s="6"/>
       <c r="C214" s="6"/>
       <c r="D214" s="6"/>
@@ -6758,7 +6801,7 @@
       <c r="Z215" s="2"/>
     </row>
     <row r="216">
-      <c r="A216" s="2"/>
+      <c r="A216" s="14"/>
       <c r="B216" s="6"/>
       <c r="C216" s="6"/>
       <c r="D216" s="6"/>
@@ -6779,7 +6822,7 @@
       <c r="S216" s="6"/>
       <c r="T216" s="6"/>
       <c r="U216" s="6"/>
-      <c r="V216" s="3"/>
+      <c r="V216" s="6"/>
       <c r="W216" s="2"/>
       <c r="X216" s="2"/>
       <c r="Y216" s="2"/>
@@ -6807,7 +6850,7 @@
       <c r="S217" s="6"/>
       <c r="T217" s="6"/>
       <c r="U217" s="6"/>
-      <c r="V217" s="3"/>
+      <c r="V217" s="6"/>
       <c r="W217" s="2"/>
       <c r="X217" s="2"/>
       <c r="Y217" s="2"/>
@@ -6835,7 +6878,7 @@
       <c r="S218" s="6"/>
       <c r="T218" s="6"/>
       <c r="U218" s="6"/>
-      <c r="V218" s="6"/>
+      <c r="V218" s="3"/>
       <c r="W218" s="2"/>
       <c r="X218" s="2"/>
       <c r="Y218" s="2"/>
@@ -6863,7 +6906,7 @@
       <c r="S219" s="6"/>
       <c r="T219" s="6"/>
       <c r="U219" s="6"/>
-      <c r="V219" s="6"/>
+      <c r="V219" s="3"/>
       <c r="W219" s="2"/>
       <c r="X219" s="2"/>
       <c r="Y219" s="2"/>
@@ -7347,27 +7390,27 @@
     </row>
     <row r="237">
       <c r="A237" s="2"/>
-      <c r="B237" s="2"/>
-      <c r="C237" s="2"/>
-      <c r="D237" s="2"/>
-      <c r="E237" s="2"/>
+      <c r="B237" s="6"/>
+      <c r="C237" s="6"/>
+      <c r="D237" s="6"/>
+      <c r="E237" s="6"/>
       <c r="F237" s="2"/>
       <c r="G237" s="2"/>
-      <c r="H237" s="2"/>
-      <c r="I237" s="2"/>
-      <c r="J237" s="2"/>
-      <c r="K237" s="2"/>
-      <c r="L237" s="2"/>
-      <c r="M237" s="2"/>
-      <c r="N237" s="2"/>
-      <c r="O237" s="2"/>
-      <c r="P237" s="2"/>
-      <c r="Q237" s="2"/>
-      <c r="R237" s="2"/>
-      <c r="S237" s="2"/>
-      <c r="T237" s="2"/>
-      <c r="U237" s="2"/>
-      <c r="V237" s="2"/>
+      <c r="H237" s="6"/>
+      <c r="I237" s="6"/>
+      <c r="J237" s="6"/>
+      <c r="K237" s="6"/>
+      <c r="L237" s="6"/>
+      <c r="M237" s="7"/>
+      <c r="N237" s="6"/>
+      <c r="O237" s="6"/>
+      <c r="P237" s="6"/>
+      <c r="Q237" s="6"/>
+      <c r="R237" s="6"/>
+      <c r="S237" s="6"/>
+      <c r="T237" s="6"/>
+      <c r="U237" s="6"/>
+      <c r="V237" s="6"/>
       <c r="W237" s="2"/>
       <c r="X237" s="2"/>
       <c r="Y237" s="2"/>
@@ -7375,27 +7418,27 @@
     </row>
     <row r="238">
       <c r="A238" s="2"/>
-      <c r="B238" s="2"/>
-      <c r="C238" s="2"/>
-      <c r="D238" s="2"/>
-      <c r="E238" s="2"/>
+      <c r="B238" s="6"/>
+      <c r="C238" s="6"/>
+      <c r="D238" s="6"/>
+      <c r="E238" s="6"/>
       <c r="F238" s="2"/>
       <c r="G238" s="2"/>
-      <c r="H238" s="2"/>
-      <c r="I238" s="2"/>
-      <c r="J238" s="2"/>
-      <c r="K238" s="2"/>
-      <c r="L238" s="2"/>
-      <c r="M238" s="2"/>
-      <c r="N238" s="2"/>
-      <c r="O238" s="2"/>
-      <c r="P238" s="2"/>
-      <c r="Q238" s="2"/>
-      <c r="R238" s="2"/>
-      <c r="S238" s="2"/>
-      <c r="T238" s="2"/>
-      <c r="U238" s="2"/>
-      <c r="V238" s="2"/>
+      <c r="H238" s="6"/>
+      <c r="I238" s="6"/>
+      <c r="J238" s="6"/>
+      <c r="K238" s="6"/>
+      <c r="L238" s="6"/>
+      <c r="M238" s="7"/>
+      <c r="N238" s="6"/>
+      <c r="O238" s="6"/>
+      <c r="P238" s="6"/>
+      <c r="Q238" s="6"/>
+      <c r="R238" s="6"/>
+      <c r="S238" s="6"/>
+      <c r="T238" s="6"/>
+      <c r="U238" s="6"/>
+      <c r="V238" s="6"/>
       <c r="W238" s="2"/>
       <c r="X238" s="2"/>
       <c r="Y238" s="2"/>
@@ -28709,6 +28752,62 @@
       <c r="Y999" s="2"/>
       <c r="Z999" s="2"/>
     </row>
+    <row r="1000">
+      <c r="A1000" s="2"/>
+      <c r="B1000" s="2"/>
+      <c r="C1000" s="2"/>
+      <c r="D1000" s="2"/>
+      <c r="E1000" s="2"/>
+      <c r="F1000" s="2"/>
+      <c r="G1000" s="2"/>
+      <c r="H1000" s="2"/>
+      <c r="I1000" s="2"/>
+      <c r="J1000" s="2"/>
+      <c r="K1000" s="2"/>
+      <c r="L1000" s="2"/>
+      <c r="M1000" s="2"/>
+      <c r="N1000" s="2"/>
+      <c r="O1000" s="2"/>
+      <c r="P1000" s="2"/>
+      <c r="Q1000" s="2"/>
+      <c r="R1000" s="2"/>
+      <c r="S1000" s="2"/>
+      <c r="T1000" s="2"/>
+      <c r="U1000" s="2"/>
+      <c r="V1000" s="2"/>
+      <c r="W1000" s="2"/>
+      <c r="X1000" s="2"/>
+      <c r="Y1000" s="2"/>
+      <c r="Z1000" s="2"/>
+    </row>
+    <row r="1001">
+      <c r="A1001" s="2"/>
+      <c r="B1001" s="2"/>
+      <c r="C1001" s="2"/>
+      <c r="D1001" s="2"/>
+      <c r="E1001" s="2"/>
+      <c r="F1001" s="2"/>
+      <c r="G1001" s="2"/>
+      <c r="H1001" s="2"/>
+      <c r="I1001" s="2"/>
+      <c r="J1001" s="2"/>
+      <c r="K1001" s="2"/>
+      <c r="L1001" s="2"/>
+      <c r="M1001" s="2"/>
+      <c r="N1001" s="2"/>
+      <c r="O1001" s="2"/>
+      <c r="P1001" s="2"/>
+      <c r="Q1001" s="2"/>
+      <c r="R1001" s="2"/>
+      <c r="S1001" s="2"/>
+      <c r="T1001" s="2"/>
+      <c r="U1001" s="2"/>
+      <c r="V1001" s="2"/>
+      <c r="W1001" s="2"/>
+      <c r="X1001" s="2"/>
+      <c r="Y1001" s="2"/>
+      <c r="Z1001" s="2"/>
+    </row>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>